<commit_message>
Update job_info and config
</commit_message>
<xml_diff>
--- a/sources/DS_Autotesting/conf/job_info.xlsx
+++ b/sources/DS_Autotesting/conf/job_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ACindy\Github\AutoTest\AutoTesting\sources\DS_AutoTesting\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95675055-4CBC-4ED1-8ACB-BFA7B0FD3AF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E285E24-F8DB-49D8-BB3B-BA13DABD01B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9072" xr2:uid="{7871E94D-3286-4398-A8DD-FCB551EE3EF4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>JOB_NAME</t>
   </si>
@@ -48,59 +48,40 @@
     <t>Sequence</t>
   </si>
   <si>
-    <t>LD_RDMSTG_GBS_RESOURCE_JobSeq</t>
-  </si>
-  <si>
-    <t>LD_RDMSTG_GBS_RES_PDA_From_XML_JobSeq</t>
-  </si>
-  <si>
-    <t>LD_RDMSTG_GBS_RES_ZOS_From_PDA_JobSeq</t>
-  </si>
-  <si>
-    <t>LD_RDMSTG_LINE_Of_BUSINESS_REFERENCE_From_XML_PJob</t>
-  </si>
-  <si>
-    <t>LD_RDMSTG_CENTER_OF_COMPETENCY_REFERENCE_From_XML_PJob</t>
-  </si>
-  <si>
     <t>Parallel</t>
   </si>
   <si>
-    <t>J500RDM01001</t>
-  </si>
-  <si>
-    <t>C500RDM01001</t>
-  </si>
-  <si>
-    <t>J500RDM01101</t>
-  </si>
-  <si>
-    <t>C500RDM01101</t>
-  </si>
-  <si>
-    <t>LD_RDMSTG_CENTER_OF_COMPETENCY_REFERENCE_ZOS_PJob</t>
-  </si>
-  <si>
-    <t>J500RDM01102</t>
-  </si>
-  <si>
-    <t>C500RDM01102</t>
-  </si>
-  <si>
-    <t>D500 CMNREF-RDM ETL 02 D ZOS | EBU Feeder Tables</t>
-  </si>
-  <si>
-    <t>D500 CMNREF-RDM ETL 01 D PDA | EBU Feeder Tables</t>
+    <t>J800801</t>
+  </si>
+  <si>
+    <t>C800801</t>
+  </si>
+  <si>
+    <t>LD_D800_Customer_JobSeq</t>
+  </si>
+  <si>
+    <t>LD_D800_JAPAN_CUSTOMER_REFERENCE_from_BMSIW_Delta_NZ_PJob</t>
+  </si>
+  <si>
+    <t>D800 CUSTOMER-BMSIW ETL 01 D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -123,16 +104,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -445,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4EAA182-23B4-4C7E-A6EF-1AABBFC86A27}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,93 +467,41 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
+      <c r="D3" t="s">
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
+      <c r="E4" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" display="LD_RDHIW_CUSTOMER_From_BMSIW_PJob@" xr:uid="{61EEC1BB-D394-4E52-ABDA-9AD5712BAFE1}"/>
+    <hyperlink ref="E2" r:id="rId2" display="http://iwrefresh.w3ibm.mybluemix.net/Domains/ODS ADL/Datagroups/D800 CUSTOMER-BMSIW ETL 01 D" xr:uid="{F2EF243F-13D4-40C7-A543-A6C0AEDF8451}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update asca and rowcount test case
</commit_message>
<xml_diff>
--- a/sources/DS_Autotesting/conf/job_info.xlsx
+++ b/sources/DS_Autotesting/conf/job_info.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ACindy\Github\AutoTest\AutoTesting\sources\DS_AutoTesting\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E285E24-F8DB-49D8-BB3B-BA13DABD01B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A441BFAF-BA56-44FE-B884-A59A460009E2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9072" xr2:uid="{7871E94D-3286-4398-A8DD-FCB551EE3EF4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7871E94D-3286-4398-A8DD-FCB551EE3EF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>JOB_NAME</t>
   </si>
@@ -51,19 +57,64 @@
     <t>Parallel</t>
   </si>
   <si>
-    <t>J800801</t>
-  </si>
-  <si>
-    <t>C800801</t>
-  </si>
-  <si>
-    <t>LD_D800_Customer_JobSeq</t>
-  </si>
-  <si>
-    <t>LD_D800_JAPAN_CUSTOMER_REFERENCE_from_BMSIW_Delta_NZ_PJob</t>
-  </si>
-  <si>
-    <t>D800 CUSTOMER-BMSIW ETL 01 D</t>
+    <t>J200104</t>
+  </si>
+  <si>
+    <t>J200105</t>
+  </si>
+  <si>
+    <t>J200106</t>
+  </si>
+  <si>
+    <t>J200108</t>
+  </si>
+  <si>
+    <t>J200109</t>
+  </si>
+  <si>
+    <t>J200110</t>
+  </si>
+  <si>
+    <t>C200104</t>
+  </si>
+  <si>
+    <t>C200105</t>
+  </si>
+  <si>
+    <t>C200106</t>
+  </si>
+  <si>
+    <t>C200108</t>
+  </si>
+  <si>
+    <t>C200109</t>
+  </si>
+  <si>
+    <t>C200110</t>
+  </si>
+  <si>
+    <t>LD_D200_Contract_Financial_JobSeq</t>
+  </si>
+  <si>
+    <t>D200 CNTRCTFI-BMSIW ETL 01 D</t>
+  </si>
+  <si>
+    <t>LD_D200_CURRENT_YEAR_REVENUE_DETAIL_COST_PJob</t>
+  </si>
+  <si>
+    <t>LD_D200_WORK_NUMBER_REVENUE_REFERENCE_PJob</t>
+  </si>
+  <si>
+    <t>LD_D200_CURRENT_MONTH_REVENUE_DETAIL_COST_PJob</t>
+  </si>
+  <si>
+    <t>LD_D200_REVENUE_COST_CURRENT_HISTORY_PJob</t>
+  </si>
+  <si>
+    <t>LD_D200_LAST_YEAR_REVENUE_COST_HISTORY_PJob</t>
+  </si>
+  <si>
+    <t>LD_D200_REVENUE_COST_CATEGORY_REFERENCE_PJob</t>
   </si>
 </sst>
 </file>
@@ -429,19 +480,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4EAA182-23B4-4C7E-A6EF-1AABBFC86A27}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="65.21875" customWidth="1"/>
+    <col min="1" max="1" width="72.33203125" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="16.44140625" customWidth="1"/>
     <col min="4" max="4" width="25.5546875" customWidth="1"/>
-    <col min="5" max="5" width="47" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" customWidth="1"/>
     <col min="6" max="6" width="56" customWidth="1"/>
   </cols>
   <sheetData>
@@ -467,18 +518,18 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -487,19 +538,102 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E4" s="1"/>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="LD_RDHIW_CUSTOMER_From_BMSIW_PJob@" xr:uid="{61EEC1BB-D394-4E52-ABDA-9AD5712BAFE1}"/>
-    <hyperlink ref="E2" r:id="rId2" display="http://iwrefresh.w3ibm.mybluemix.net/Domains/ODS ADL/Datagroups/D800 CUSTOMER-BMSIW ETL 01 D" xr:uid="{F2EF243F-13D4-40C7-A543-A6C0AEDF8451}"/>
+    <hyperlink ref="E2" r:id="rId1" display="http://iwrefresh.w3ibm.mybluemix.net/Domains/ODS ADL/Datagroups/D800 CUSTOMER-BMSIW ETL 01 D" xr:uid="{F2EF243F-13D4-40C7-A543-A6C0AEDF8451}"/>
+    <hyperlink ref="A3" r:id="rId2" display="LD_D200_REVENUE_COST_CATEGORY_REFERENCE_PJob@J200104@C200104" xr:uid="{5222810F-2BDA-4090-975E-59D6B9E0F4A0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>